<commit_message>
updated solar lci sheet
</commit_message>
<xml_diff>
--- a/data/inputs/layered oxide cathode type_HC anode SIB .xlsx
+++ b/data/inputs/layered oxide cathode type_HC anode SIB .xlsx
@@ -457,9 +457,6 @@
     <t>printed wiring board, for through-hole mounting, Pb free surface</t>
   </si>
   <si>
-    <t>m</t>
-  </si>
-  <si>
     <t>market for cable, data cable in infrastructure</t>
   </si>
   <si>
@@ -527,6 +524,9 @@
   </si>
   <si>
     <t>market for lime, hydrated, loose weight</t>
+  </si>
+  <si>
+    <t>meter</t>
   </si>
 </sst>
 </file>
@@ -995,9 +995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A261" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F272" sqref="F272"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1021,10 +1019,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" t="s">
         <v>146</v>
-      </c>
-      <c r="B2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1041,7 +1039,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1097,7 +1095,7 @@
         <v>10</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1171,7 +1169,7 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1227,7 +1225,7 @@
         <v>10</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -1282,7 +1280,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B24">
         <v>2.12E-2</v>
@@ -1291,7 +1289,7 @@
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F24" t="s">
         <v>13</v>
@@ -1364,7 +1362,7 @@
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F27" t="s">
         <v>12</v>
@@ -1387,7 +1385,7 @@
         <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F28" t="s">
         <v>12</v>
@@ -1407,10 +1405,10 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="C29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F29" t="s">
         <v>14</v>
@@ -1430,10 +1428,10 @@
         <v>0.25</v>
       </c>
       <c r="C30" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F30" t="s">
         <v>12</v>
@@ -1453,10 +1451,10 @@
         <v>3.64</v>
       </c>
       <c r="C31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D31" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F31" t="s">
         <v>37</v>
@@ -1476,10 +1474,10 @@
         <v>26.31</v>
       </c>
       <c r="C32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F32" t="s">
         <v>12</v>
@@ -1499,13 +1497,13 @@
         <v>0.46899999999999997</v>
       </c>
       <c r="C33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E33" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G33" t="s">
         <v>15</v>
@@ -1522,7 +1520,7 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F34" t="s">
         <v>13</v>
@@ -1554,7 +1552,7 @@
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -1610,7 +1608,7 @@
         <v>10</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -1649,7 +1647,7 @@
         <v>4</v>
       </c>
       <c r="D45" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F45" t="s">
         <v>13</v>
@@ -1672,7 +1670,7 @@
         <v>4</v>
       </c>
       <c r="D46" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F46" t="s">
         <v>13</v>
@@ -1686,7 +1684,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B47" s="5">
         <v>1.8200000000000001E-2</v>
@@ -1695,10 +1693,10 @@
         <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G47" t="s">
         <v>11</v>
@@ -1718,7 +1716,7 @@
         <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F48" t="s">
         <v>13</v>
@@ -1738,10 +1736,10 @@
         <v>1.49E-2</v>
       </c>
       <c r="C49" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D49" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F49" t="s">
         <v>12</v>
@@ -1761,10 +1759,10 @@
         <v>5.28E-2</v>
       </c>
       <c r="C50" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D50" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F50" t="s">
         <v>12</v>
@@ -1787,7 +1785,7 @@
         <v>3</v>
       </c>
       <c r="D51" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F51" t="s">
         <v>12</v>
@@ -1807,10 +1805,10 @@
         <v>2E-3</v>
       </c>
       <c r="C52" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D52" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F52" t="s">
         <v>37</v>
@@ -1824,16 +1822,16 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B53" s="5">
         <v>0.26700000000000002</v>
       </c>
       <c r="C53" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D53" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F53" t="s">
         <v>28</v>
@@ -1853,13 +1851,13 @@
         <v>0.26700000000000002</v>
       </c>
       <c r="C54" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D54" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G54" t="s">
         <v>15</v>
@@ -1885,7 +1883,7 @@
         <v>10</v>
       </c>
       <c r="B59" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
@@ -1941,7 +1939,7 @@
         <v>10</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
@@ -1955,7 +1953,7 @@
         <v>4</v>
       </c>
       <c r="D65" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F65" t="s">
         <v>13</v>
@@ -1978,7 +1976,7 @@
         <v>4</v>
       </c>
       <c r="D66" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F66" t="s">
         <v>13</v>
@@ -2051,7 +2049,7 @@
         <v>4</v>
       </c>
       <c r="D69" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F69" t="s">
         <v>12</v>
@@ -2071,10 +2069,10 @@
         <v>0.13600000000000001</v>
       </c>
       <c r="C70" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D70" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F70" t="s">
         <v>12</v>
@@ -2094,10 +2092,10 @@
         <v>0.81699999999999995</v>
       </c>
       <c r="C71" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D71" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F71" t="s">
         <v>12</v>
@@ -2120,7 +2118,7 @@
         <v>3</v>
       </c>
       <c r="D72" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F72" t="s">
         <v>12</v>
@@ -2138,10 +2136,10 @@
         <v>3.0800000000000001E-2</v>
       </c>
       <c r="C73" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D73" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F73" t="s">
         <v>37</v>
@@ -2153,16 +2151,16 @@
     </row>
     <row r="74" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B74" s="5">
         <v>10.6</v>
       </c>
       <c r="C74" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D74" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F74" t="s">
         <v>28</v>
@@ -2183,7 +2181,7 @@
         <v>4</v>
       </c>
       <c r="D75" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G75" t="s">
         <v>15</v>
@@ -2198,13 +2196,13 @@
         <v>10.71</v>
       </c>
       <c r="C76" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D76" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E76" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G76" t="s">
         <v>15</v>
@@ -2235,7 +2233,7 @@
         <v>10</v>
       </c>
       <c r="B80" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
@@ -2296,7 +2294,7 @@
         <v>10</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
@@ -2310,7 +2308,7 @@
         <v>4</v>
       </c>
       <c r="D86" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F86" t="s">
         <v>13</v>
@@ -2333,7 +2331,7 @@
         <v>4</v>
       </c>
       <c r="D87" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F87" t="s">
         <v>13</v>
@@ -2356,7 +2354,7 @@
         <v>4</v>
       </c>
       <c r="D88" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F88" t="s">
         <v>28</v>
@@ -2376,10 +2374,10 @@
         <v>0.27200000000000002</v>
       </c>
       <c r="C89" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D89" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F89" t="s">
         <v>14</v>
@@ -2399,10 +2397,10 @@
         <v>1.63</v>
       </c>
       <c r="C90" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D90" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F90" t="s">
         <v>12</v>
@@ -2422,10 +2420,10 @@
         <v>1.12E-2</v>
       </c>
       <c r="C91" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D91" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F91" t="s">
         <v>14</v>
@@ -2437,16 +2435,16 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B92" s="5">
         <v>2.62</v>
       </c>
       <c r="C92" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D92" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F92" t="s">
         <v>28</v>
@@ -2467,7 +2465,7 @@
         <v>4</v>
       </c>
       <c r="D93" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G93" t="s">
         <v>15</v>
@@ -2482,10 +2480,10 @@
         <v>2.29</v>
       </c>
       <c r="C94" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D94" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G94" t="s">
         <v>15</v>
@@ -2503,10 +2501,10 @@
         <v>4</v>
       </c>
       <c r="D95" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E95" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G95" t="s">
         <v>15</v>
@@ -2523,10 +2521,10 @@
         <v>4</v>
       </c>
       <c r="D96" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E96" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G96" t="s">
         <v>15</v>
@@ -2543,10 +2541,10 @@
         <v>4</v>
       </c>
       <c r="D97" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E97" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G97" t="s">
         <v>15</v>
@@ -2563,10 +2561,10 @@
         <v>4</v>
       </c>
       <c r="D98" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E98" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G98" t="s">
         <v>15</v>
@@ -2595,7 +2593,7 @@
         <v>10</v>
       </c>
       <c r="B103" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
@@ -2657,7 +2655,7 @@
         <v>10</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.3">
@@ -2671,7 +2669,7 @@
         <v>4</v>
       </c>
       <c r="D109" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F109" t="s">
         <v>13</v>
@@ -2685,7 +2683,7 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B110" s="15">
         <v>1.2</v>
@@ -2694,7 +2692,7 @@
         <v>4</v>
       </c>
       <c r="D110" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E110" s="4"/>
       <c r="F110" t="s">
@@ -2715,10 +2713,10 @@
         <v>0.27200000000000002</v>
       </c>
       <c r="C111" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D111" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F111" t="s">
         <v>12</v>
@@ -2738,10 +2736,10 @@
         <v>0.71699999999999997</v>
       </c>
       <c r="C112" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D112" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F112" t="s">
         <v>12</v>
@@ -2761,10 +2759,10 @@
         <v>1.78</v>
       </c>
       <c r="C113" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D113" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F113" t="s">
         <v>37</v>
@@ -2782,13 +2780,13 @@
         <v>6.42</v>
       </c>
       <c r="C114" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D114" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E114" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G114" t="s">
         <v>15</v>
@@ -2814,7 +2812,7 @@
         <v>10</v>
       </c>
       <c r="B118" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.3">
@@ -2903,7 +2901,7 @@
         <v>4</v>
       </c>
       <c r="D125" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F125" t="s">
         <v>13</v>
@@ -2926,7 +2924,7 @@
         <v>4</v>
       </c>
       <c r="D126" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F126" t="s">
         <v>13</v>
@@ -2949,7 +2947,7 @@
         <v>4</v>
       </c>
       <c r="D127" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F127" t="s">
         <v>37</v>
@@ -2969,7 +2967,7 @@
         <v>4</v>
       </c>
       <c r="D128" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F128" t="s">
         <v>28</v>
@@ -2992,7 +2990,7 @@
         <v>4</v>
       </c>
       <c r="D129" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F129" t="s">
         <v>13</v>
@@ -3015,7 +3013,7 @@
         <v>4</v>
       </c>
       <c r="D130" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F130" t="s">
         <v>13</v>
@@ -3035,10 +3033,10 @@
         <v>1.8800000000000001E-2</v>
       </c>
       <c r="C131" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D131" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F131" t="s">
         <v>14</v>
@@ -3058,10 +3056,10 @@
         <v>5.7700000000000001E-2</v>
       </c>
       <c r="C132" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D132" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F132" t="s">
         <v>12</v>
@@ -3084,7 +3082,7 @@
         <v>3</v>
       </c>
       <c r="D133" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F133" t="s">
         <v>12</v>
@@ -3104,13 +3102,13 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="C134" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D134" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E134" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G134" t="s">
         <v>15</v>
@@ -3127,7 +3125,7 @@
         <v>4</v>
       </c>
       <c r="D135" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G135" t="s">
         <v>15</v>
@@ -3150,7 +3148,7 @@
         <v>10</v>
       </c>
       <c r="B138" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.3">
@@ -3203,7 +3201,7 @@
         <v>10</v>
       </c>
       <c r="H143" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.3">
@@ -3217,7 +3215,7 @@
         <v>4</v>
       </c>
       <c r="D144" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F144" t="s">
         <v>13</v>
@@ -3237,10 +3235,10 @@
         <v>0.107</v>
       </c>
       <c r="C145" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D145" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F145" t="s">
         <v>37</v>
@@ -3260,10 +3258,10 @@
         <v>9.52</v>
       </c>
       <c r="C146" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D146" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F146" t="s">
         <v>28</v>
@@ -3286,7 +3284,7 @@
         <v>4</v>
       </c>
       <c r="D147" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F147" t="s">
         <v>28</v>
@@ -3309,7 +3307,7 @@
         <v>4</v>
       </c>
       <c r="D148" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F148" t="s">
         <v>13</v>
@@ -3332,7 +3330,7 @@
         <v>4</v>
       </c>
       <c r="D149" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F149" t="s">
         <v>12</v>
@@ -3352,10 +3350,10 @@
         <v>1.38</v>
       </c>
       <c r="C150" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D150" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F150" t="s">
         <v>12</v>
@@ -3375,10 +3373,10 @@
         <v>4.8600000000000003</v>
       </c>
       <c r="C151" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D151" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F151" t="s">
         <v>13</v>
@@ -3401,7 +3399,7 @@
         <v>35</v>
       </c>
       <c r="D152" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F152" t="s">
         <v>12</v>
@@ -3424,7 +3422,7 @@
         <v>4</v>
       </c>
       <c r="D153" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G153" t="s">
         <v>15</v>
@@ -3441,7 +3439,7 @@
         <v>4</v>
       </c>
       <c r="D154" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G154" t="s">
         <v>15</v>
@@ -3458,7 +3456,7 @@
         <v>4</v>
       </c>
       <c r="D155" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G155" t="s">
         <v>15</v>
@@ -3475,7 +3473,7 @@
         <v>4</v>
       </c>
       <c r="D156" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G156" t="s">
         <v>15</v>
@@ -3492,7 +3490,7 @@
         <v>4</v>
       </c>
       <c r="D157" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G157" t="s">
         <v>15</v>
@@ -3509,7 +3507,7 @@
         <v>4</v>
       </c>
       <c r="D158" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G158" t="s">
         <v>15</v>
@@ -3526,7 +3524,7 @@
         <v>4</v>
       </c>
       <c r="D159" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G159" t="s">
         <v>15</v>
@@ -3543,7 +3541,7 @@
         <v>4</v>
       </c>
       <c r="D160" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G160" t="s">
         <v>15</v>
@@ -3557,13 +3555,13 @@
         <v>9.9</v>
       </c>
       <c r="C161" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D161" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E161" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G161" t="s">
         <v>15</v>
@@ -3581,7 +3579,7 @@
         <v>4</v>
       </c>
       <c r="D162" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F162" t="s">
         <v>37</v>
@@ -3601,10 +3599,10 @@
         <v>1.78E-2</v>
       </c>
       <c r="C163" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D163" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F163" t="s">
         <v>28</v>
@@ -3636,7 +3634,7 @@
         <v>10</v>
       </c>
       <c r="B167" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.3">
@@ -3704,7 +3702,7 @@
         <v>4</v>
       </c>
       <c r="D173" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F173" t="s">
         <v>12</v>
@@ -3727,7 +3725,7 @@
         <v>4</v>
       </c>
       <c r="D174" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F174" t="s">
         <v>28</v>
@@ -3750,7 +3748,7 @@
         <v>4</v>
       </c>
       <c r="D175" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F175" t="s">
         <v>13</v>
@@ -3773,7 +3771,7 @@
         <v>4</v>
       </c>
       <c r="D176" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F176" t="s">
         <v>13</v>
@@ -3787,7 +3785,7 @@
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B177" s="5">
         <v>0.01</v>
@@ -3796,7 +3794,7 @@
         <v>4</v>
       </c>
       <c r="D177" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F177" t="s">
         <v>13</v>
@@ -3819,7 +3817,7 @@
         <v>4</v>
       </c>
       <c r="D178" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F178" t="s">
         <v>13</v>
@@ -3842,10 +3840,10 @@
         <v>3</v>
       </c>
       <c r="D179" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F179" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G179" t="s">
         <v>11</v>
@@ -3865,7 +3863,7 @@
         <v>4</v>
       </c>
       <c r="D180" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F180" t="s">
         <v>13</v>
@@ -3885,10 +3883,10 @@
         <v>0.105</v>
       </c>
       <c r="C181" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D181" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F181" t="s">
         <v>12</v>
@@ -3908,10 +3906,10 @@
         <v>0.627</v>
       </c>
       <c r="C182" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D182" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F182" t="s">
         <v>12</v>
@@ -3931,10 +3929,10 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="C183" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D183" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F183" t="s">
         <v>37</v>
@@ -3954,10 +3952,10 @@
         <v>13.75</v>
       </c>
       <c r="C184" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D184" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F184" t="s">
         <v>12</v>
@@ -3980,7 +3978,7 @@
         <v>3</v>
       </c>
       <c r="D185" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F185" t="s">
         <v>12</v>
@@ -4000,13 +3998,13 @@
         <v>15.73</v>
       </c>
       <c r="C186" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D186" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E186" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G186" t="s">
         <v>15</v>
@@ -4023,7 +4021,7 @@
         <v>4</v>
       </c>
       <c r="D187" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G187" t="s">
         <v>15</v>
@@ -4049,7 +4047,7 @@
         <v>10</v>
       </c>
       <c r="B192" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.3">
@@ -4114,7 +4112,7 @@
         <v>4</v>
       </c>
       <c r="D198" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F198" t="s">
         <v>13</v>
@@ -4137,7 +4135,7 @@
         <v>4</v>
       </c>
       <c r="D199" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F199" t="s">
         <v>13</v>
@@ -4182,10 +4180,10 @@
         <v>0.1</v>
       </c>
       <c r="C201" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D201" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F201" t="s">
         <v>12</v>
@@ -4205,10 +4203,10 @@
         <v>0.6</v>
       </c>
       <c r="C202" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D202" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F202" t="s">
         <v>12</v>
@@ -4244,7 +4242,7 @@
         <v>10</v>
       </c>
       <c r="B206" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.3">
@@ -4312,7 +4310,7 @@
         <v>4</v>
       </c>
       <c r="D212" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F212" t="s">
         <v>13</v>
@@ -4335,7 +4333,7 @@
         <v>4</v>
       </c>
       <c r="D213" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F213" t="s">
         <v>13</v>
@@ -4358,7 +4356,7 @@
         <v>4</v>
       </c>
       <c r="D214" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F214" t="s">
         <v>12</v>
@@ -4381,7 +4379,7 @@
         <v>4</v>
       </c>
       <c r="D215" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F215" t="s">
         <v>12</v>
@@ -4404,7 +4402,7 @@
         <v>4</v>
       </c>
       <c r="D216" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F216" t="s">
         <v>12</v>
@@ -4424,10 +4422,10 @@
         <v>0.1</v>
       </c>
       <c r="C217" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D217" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F217" t="s">
         <v>12</v>
@@ -4447,10 +4445,10 @@
         <v>0.6</v>
       </c>
       <c r="C218" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D218" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F218" t="s">
         <v>28</v>
@@ -4473,7 +4471,7 @@
         <v>51</v>
       </c>
       <c r="D219" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F219" t="s">
         <v>12</v>
@@ -4496,7 +4494,7 @@
         <v>4</v>
       </c>
       <c r="D220" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G220" t="s">
         <v>15</v>
@@ -4511,13 +4509,13 @@
         <v>1.95</v>
       </c>
       <c r="C221" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D221" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E221" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G221" t="s">
         <v>15</v>
@@ -4534,7 +4532,7 @@
         <v>4</v>
       </c>
       <c r="D222" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F222" t="s">
         <v>14</v>
@@ -4554,10 +4552,10 @@
         <v>3.6099999999999999E-3</v>
       </c>
       <c r="C223" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D223" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F223" t="s">
         <v>14</v>
@@ -4588,7 +4586,7 @@
         <v>10</v>
       </c>
       <c r="B227" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.3">
@@ -4653,7 +4651,7 @@
         <v>4</v>
       </c>
       <c r="D233" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F233" t="s">
         <v>13</v>
@@ -4676,7 +4674,7 @@
         <v>4</v>
       </c>
       <c r="D234" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F234" t="s">
         <v>13</v>
@@ -4699,7 +4697,7 @@
         <v>4</v>
       </c>
       <c r="D235" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F235" t="s">
         <v>14</v>
@@ -4719,10 +4717,10 @@
         <v>0.2</v>
       </c>
       <c r="C236" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D236" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F236" t="s">
         <v>13</v>
@@ -4742,10 +4740,10 @@
         <v>1.2</v>
       </c>
       <c r="C237" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D237" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F237" t="s">
         <v>13</v>
@@ -4768,7 +4766,7 @@
         <v>3</v>
       </c>
       <c r="D238" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F238" t="s">
         <v>13</v>
@@ -4799,7 +4797,7 @@
         <v>10</v>
       </c>
       <c r="B243" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.3">
@@ -4867,7 +4865,7 @@
         <v>4</v>
       </c>
       <c r="D249" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F249" t="s">
         <v>13</v>
@@ -4890,7 +4888,7 @@
         <v>4</v>
       </c>
       <c r="D250" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F250" t="s">
         <v>12</v>
@@ -4935,7 +4933,7 @@
         <v>51</v>
       </c>
       <c r="D252" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F252" t="s">
         <v>12</v>
@@ -4955,10 +4953,10 @@
         <v>0.1</v>
       </c>
       <c r="C253" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D253" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F253" t="s">
         <v>12</v>
@@ -4978,10 +4976,10 @@
         <v>0.54200000000000004</v>
       </c>
       <c r="C254" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D254" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F254" t="s">
         <v>28</v>
@@ -5001,10 +4999,10 @@
         <v>3.53</v>
       </c>
       <c r="C255" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D255" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F255" t="s">
         <v>37</v>
@@ -5024,13 +5022,13 @@
         <v>12.72</v>
       </c>
       <c r="C256" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D256" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E256" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G256" t="s">
         <v>15</v>
@@ -5050,7 +5048,7 @@
         <v>10</v>
       </c>
       <c r="B260" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.3">
@@ -5109,7 +5107,7 @@
     </row>
     <row r="266" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A266" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B266" s="5">
         <v>1.8100000000000002E-2</v>
@@ -5118,7 +5116,7 @@
         <v>4</v>
       </c>
       <c r="D266" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F266" t="s">
         <v>13</v>
@@ -5141,7 +5139,7 @@
         <v>4</v>
       </c>
       <c r="D267" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F267" t="s">
         <v>13</v>
@@ -5155,16 +5153,16 @@
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A268" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B268" s="5">
         <v>6.66</v>
       </c>
       <c r="C268" t="s">
-        <v>141</v>
+        <v>164</v>
       </c>
       <c r="D268" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F268" t="s">
         <v>13</v>
@@ -5173,21 +5171,21 @@
         <v>11</v>
       </c>
       <c r="H268" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="269" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A269" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B269" s="5">
         <v>0.44600000000000001</v>
       </c>
       <c r="C269" t="s">
-        <v>141</v>
+        <v>164</v>
       </c>
       <c r="D269" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F269" t="s">
         <v>13</v>
@@ -5196,7 +5194,7 @@
         <v>11</v>
       </c>
       <c r="H269" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="270" spans="1:8" x14ac:dyDescent="0.3">
@@ -5207,10 +5205,10 @@
         <v>9.3956999999999999E-2</v>
       </c>
       <c r="C270" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D270" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F270" t="s">
         <v>12</v>
@@ -5230,10 +5228,10 @@
         <v>0.56374000000000002</v>
       </c>
       <c r="C271" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D271" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F271" t="s">
         <v>28</v>
@@ -5406,18 +5404,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5439,14 +5437,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC7C0EC8-0C3B-44A9-8033-00137DC09A49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5855932F-2918-4696-B2D1-0ED741520C0F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -5460,4 +5450,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC7C0EC8-0C3B-44A9-8033-00137DC09A49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>